<commit_message>
dl notes added. python notes updated.
</commit_message>
<xml_diff>
--- a/Learning_Topics.xlsx
+++ b/Learning_Topics.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Papers" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1558,18 +1557,57 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1579,62 +1617,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1990,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -2127,7 +2126,7 @@
       <c r="C13" s="35"/>
       <c r="D13" s="36"/>
       <c r="E13" s="40"/>
-      <c r="F13" s="61"/>
+      <c r="F13" s="48"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="34"/>
@@ -2161,65 +2160,65 @@
     <row r="18" spans="3:6" ht="15" thickBot="1">
       <c r="D18" s="36"/>
       <c r="E18" s="37"/>
-      <c r="F18" s="61"/>
+      <c r="F18" s="48"/>
     </row>
     <row r="19" spans="3:6" ht="43.2">
-      <c r="C19" s="65" t="s">
+      <c r="C19" s="53" t="s">
         <v>277</v>
       </c>
-      <c r="D19" s="62" t="s">
+      <c r="D19" s="49" t="s">
         <v>278</v>
       </c>
-      <c r="E19" s="63" t="s">
+      <c r="E19" s="50" t="s">
         <v>279</v>
       </c>
-      <c r="F19" s="64" t="s">
+      <c r="F19" s="51" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="20" spans="3:6">
-      <c r="C20" s="66"/>
-      <c r="D20" s="62" t="s">
+      <c r="C20" s="54"/>
+      <c r="D20" s="49" t="s">
         <v>288</v>
       </c>
-      <c r="E20" s="63"/>
-      <c r="F20" s="64"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="51"/>
     </row>
     <row r="21" spans="3:6">
-      <c r="C21" s="66"/>
-      <c r="D21" s="62" t="s">
+      <c r="C21" s="54"/>
+      <c r="D21" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="63" t="s">
+      <c r="E21" s="50" t="s">
         <v>282</v>
       </c>
-      <c r="F21" s="64" t="s">
+      <c r="F21" s="51" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="22" spans="3:6">
-      <c r="C22" s="66"/>
-      <c r="D22" s="62" t="s">
+      <c r="C22" s="54"/>
+      <c r="D22" s="49" t="s">
         <v>283</v>
       </c>
-      <c r="E22" s="63" t="s">
+      <c r="E22" s="50" t="s">
         <v>284</v>
       </c>
-      <c r="F22" s="64" t="s">
+      <c r="F22" s="51" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="23" spans="3:6">
-      <c r="C23" s="66"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="64"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="51"/>
     </row>
     <row r="24" spans="3:6" ht="15" thickBot="1">
-      <c r="C24" s="67"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="64"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="51"/>
     </row>
     <row r="25" spans="3:6">
       <c r="F25" s="7"/>
@@ -2228,473 +2227,473 @@
       <c r="F26" s="7"/>
     </row>
     <row r="27" spans="3:6" ht="28.8">
-      <c r="D27" s="62" t="s">
+      <c r="D27" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="63"/>
-      <c r="F27" s="64" t="s">
+      <c r="E27" s="50"/>
+      <c r="F27" s="51" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="3:6" ht="28.8">
-      <c r="D28" s="62" t="s">
+      <c r="D28" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="63"/>
-      <c r="F28" s="64" t="s">
+      <c r="E28" s="50"/>
+      <c r="F28" s="51" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="3:6">
       <c r="D29" s="36"/>
       <c r="E29" s="37"/>
-      <c r="F29" s="61"/>
+      <c r="F29" s="48"/>
     </row>
     <row r="30" spans="3:6" ht="15" thickBot="1">
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="3:6" ht="100.8">
-      <c r="C31" s="65" t="s">
+      <c r="C31" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="D31" s="62" t="s">
+      <c r="D31" s="49" t="s">
         <v>161</v>
       </c>
-      <c r="E31" s="63" t="s">
+      <c r="E31" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="F31" s="64" t="s">
+      <c r="F31" s="51" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="32" spans="3:6" ht="100.8">
-      <c r="C32" s="66"/>
-      <c r="D32" s="62" t="s">
+      <c r="C32" s="54"/>
+      <c r="D32" s="49" t="s">
         <v>163</v>
       </c>
-      <c r="E32" s="63" t="s">
+      <c r="E32" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="F32" s="64" t="s">
+      <c r="F32" s="51" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="33" spans="3:6" ht="172.8">
-      <c r="C33" s="66"/>
-      <c r="D33" s="62" t="s">
+      <c r="C33" s="54"/>
+      <c r="D33" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="E33" s="63" t="s">
+      <c r="E33" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="F33" s="64" t="s">
+      <c r="F33" s="51" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="34" spans="3:6" ht="28.8">
-      <c r="C34" s="66"/>
-      <c r="D34" s="62" t="s">
+      <c r="C34" s="54"/>
+      <c r="D34" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="E34" s="63"/>
-      <c r="F34" s="64" t="s">
+      <c r="E34" s="50"/>
+      <c r="F34" s="51" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="35" spans="3:6" ht="100.8">
-      <c r="C35" s="66"/>
-      <c r="D35" s="62" t="s">
+      <c r="C35" s="54"/>
+      <c r="D35" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="E35" s="63" t="s">
+      <c r="E35" s="50" t="s">
         <v>214</v>
       </c>
-      <c r="F35" s="64" t="s">
+      <c r="F35" s="51" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="36" spans="3:6" ht="201.6">
-      <c r="C36" s="66"/>
-      <c r="D36" s="62" t="s">
+      <c r="C36" s="54"/>
+      <c r="D36" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="E36" s="63" t="s">
+      <c r="E36" s="50" t="s">
         <v>208</v>
       </c>
-      <c r="F36" s="64" t="s">
+      <c r="F36" s="51" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="37" spans="3:6" ht="172.8">
-      <c r="C37" s="66"/>
-      <c r="D37" s="62" t="s">
+      <c r="C37" s="54"/>
+      <c r="D37" s="49" t="s">
         <v>209</v>
       </c>
-      <c r="E37" s="63" t="s">
+      <c r="E37" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="F37" s="64" t="s">
+      <c r="F37" s="51" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="38" spans="3:6">
-      <c r="C38" s="66"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="64"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="51"/>
     </row>
     <row r="39" spans="3:6" ht="15" thickBot="1">
-      <c r="C39" s="67"/>
-      <c r="D39" s="62"/>
-      <c r="E39" s="63"/>
-      <c r="F39" s="64"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="51"/>
     </row>
     <row r="40" spans="3:6" ht="15" thickBot="1">
       <c r="C40" s="35"/>
       <c r="F40" s="7"/>
     </row>
     <row r="41" spans="3:6" ht="86.4">
-      <c r="C41" s="65" t="s">
+      <c r="C41" s="53" t="s">
         <v>217</v>
       </c>
-      <c r="D41" s="63"/>
-      <c r="E41" s="63" t="s">
+      <c r="D41" s="50"/>
+      <c r="E41" s="50" t="s">
         <v>238</v>
       </c>
-      <c r="F41" s="64" t="s">
+      <c r="F41" s="51" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="42" spans="3:6" ht="72">
-      <c r="C42" s="66"/>
-      <c r="D42" s="62" t="s">
+      <c r="C42" s="54"/>
+      <c r="D42" s="49" t="s">
         <v>204</v>
       </c>
-      <c r="E42" s="63" t="s">
+      <c r="E42" s="50" t="s">
         <v>241</v>
       </c>
-      <c r="F42" s="64" t="s">
+      <c r="F42" s="51" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="43" spans="3:6" ht="57.6">
-      <c r="C43" s="66"/>
-      <c r="D43" s="62" t="s">
+      <c r="C43" s="54"/>
+      <c r="D43" s="49" t="s">
         <v>242</v>
       </c>
-      <c r="E43" s="63" t="s">
+      <c r="E43" s="50" t="s">
         <v>243</v>
       </c>
-      <c r="F43" s="64" t="s">
+      <c r="F43" s="51" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="44" spans="3:6" ht="115.2">
-      <c r="C44" s="68"/>
-      <c r="D44" s="62" t="s">
+      <c r="C44" s="58"/>
+      <c r="D44" s="49" t="s">
         <v>205</v>
       </c>
-      <c r="E44" s="63" t="s">
+      <c r="E44" s="50" t="s">
         <v>246</v>
       </c>
-      <c r="F44" s="64" t="s">
+      <c r="F44" s="51" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="45" spans="3:6" ht="29.4" thickBot="1">
-      <c r="C45" s="69"/>
-      <c r="D45" s="62" t="s">
+      <c r="C45" s="59"/>
+      <c r="D45" s="49" t="s">
         <v>216</v>
       </c>
-      <c r="E45" s="63"/>
-      <c r="F45" s="64"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="51"/>
     </row>
     <row r="46" spans="3:6" ht="15" thickBot="1">
       <c r="C46" s="35"/>
       <c r="F46" s="7"/>
     </row>
     <row r="47" spans="3:6" ht="72">
-      <c r="C47" s="65" t="s">
+      <c r="C47" s="53" t="s">
         <v>219</v>
       </c>
-      <c r="D47" s="63"/>
-      <c r="E47" s="63" t="s">
+      <c r="D47" s="50"/>
+      <c r="E47" s="50" t="s">
         <v>268</v>
       </c>
-      <c r="F47" s="64" t="s">
+      <c r="F47" s="51" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="48" spans="3:6">
-      <c r="C48" s="66"/>
-      <c r="D48" s="62" t="s">
+      <c r="C48" s="54"/>
+      <c r="D48" s="49" t="s">
         <v>266</v>
       </c>
-      <c r="E48" s="63"/>
-      <c r="F48" s="64"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="51"/>
     </row>
     <row r="49" spans="3:6">
-      <c r="C49" s="66"/>
-      <c r="D49" s="62" t="s">
+      <c r="C49" s="54"/>
+      <c r="D49" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="E49" s="63"/>
-      <c r="F49" s="64"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="51"/>
     </row>
     <row r="50" spans="3:6" ht="28.8">
-      <c r="C50" s="66"/>
-      <c r="D50" s="62" t="s">
+      <c r="C50" s="54"/>
+      <c r="D50" s="49" t="s">
         <v>220</v>
       </c>
-      <c r="E50" s="63"/>
-      <c r="F50" s="64"/>
+      <c r="E50" s="50"/>
+      <c r="F50" s="51"/>
     </row>
     <row r="51" spans="3:6" ht="43.8" thickBot="1">
-      <c r="C51" s="69"/>
-      <c r="D51" s="62" t="s">
+      <c r="C51" s="59"/>
+      <c r="D51" s="49" t="s">
         <v>269</v>
       </c>
-      <c r="E51" s="63" t="s">
+      <c r="E51" s="50" t="s">
         <v>270</v>
       </c>
-      <c r="F51" s="64"/>
+      <c r="F51" s="51"/>
     </row>
     <row r="52" spans="3:6" ht="15" thickBot="1">
       <c r="C52" s="35"/>
       <c r="F52" s="7"/>
     </row>
     <row r="53" spans="3:6" ht="28.8">
-      <c r="C53" s="65" t="s">
+      <c r="C53" s="53" t="s">
         <v>221</v>
       </c>
-      <c r="D53" s="63"/>
-      <c r="E53" s="63" t="s">
+      <c r="D53" s="50"/>
+      <c r="E53" s="50" t="s">
         <v>222</v>
       </c>
-      <c r="F53" s="64" t="s">
+      <c r="F53" s="51" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="54" spans="3:6">
-      <c r="C54" s="66"/>
-      <c r="D54" s="62" t="s">
+      <c r="C54" s="54"/>
+      <c r="D54" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="E54" s="63"/>
-      <c r="F54" s="64"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="51"/>
     </row>
     <row r="55" spans="3:6" ht="15" thickBot="1">
-      <c r="C55" s="69"/>
-      <c r="D55" s="62" t="s">
+      <c r="C55" s="59"/>
+      <c r="D55" s="49" t="s">
         <v>223</v>
       </c>
-      <c r="E55" s="63"/>
-      <c r="F55" s="64"/>
+      <c r="E55" s="50"/>
+      <c r="F55" s="51"/>
     </row>
     <row r="56" spans="3:6" ht="15" thickBot="1">
       <c r="C56" s="35"/>
       <c r="F56" s="7"/>
     </row>
     <row r="57" spans="3:6" ht="28.8">
-      <c r="C57" s="65" t="s">
+      <c r="C57" s="53" t="s">
         <v>224</v>
       </c>
-      <c r="D57" s="63"/>
-      <c r="E57" s="63" t="s">
+      <c r="D57" s="50"/>
+      <c r="E57" s="50" t="s">
         <v>225</v>
       </c>
-      <c r="F57" s="64" t="s">
+      <c r="F57" s="51" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="58" spans="3:6" ht="115.2">
-      <c r="C58" s="66"/>
-      <c r="D58" s="62" t="s">
+      <c r="C58" s="54"/>
+      <c r="D58" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="E58" s="63" t="s">
+      <c r="E58" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="F58" s="64"/>
+      <c r="F58" s="51"/>
     </row>
     <row r="59" spans="3:6" ht="15" thickBot="1">
-      <c r="C59" s="69"/>
-      <c r="D59" s="62"/>
-      <c r="E59" s="63"/>
-      <c r="F59" s="64"/>
+      <c r="C59" s="59"/>
+      <c r="D59" s="49"/>
+      <c r="E59" s="50"/>
+      <c r="F59" s="51"/>
     </row>
     <row r="60" spans="3:6" ht="15" thickBot="1">
       <c r="C60" s="35"/>
       <c r="F60" s="7"/>
     </row>
     <row r="61" spans="3:6" ht="28.8">
-      <c r="C61" s="65" t="s">
+      <c r="C61" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="D61" s="63"/>
-      <c r="E61" s="63" t="s">
+      <c r="D61" s="50"/>
+      <c r="E61" s="50" t="s">
         <v>228</v>
       </c>
-      <c r="F61" s="64" t="s">
+      <c r="F61" s="51" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="62" spans="3:6" ht="28.8">
-      <c r="C62" s="66"/>
-      <c r="D62" s="62" t="s">
+      <c r="C62" s="54"/>
+      <c r="D62" s="49" t="s">
         <v>227</v>
       </c>
-      <c r="E62" s="63"/>
-      <c r="F62" s="64"/>
+      <c r="E62" s="50"/>
+      <c r="F62" s="51"/>
     </row>
     <row r="63" spans="3:6" ht="15" thickBot="1">
-      <c r="C63" s="69"/>
-      <c r="D63" s="62"/>
-      <c r="E63" s="63"/>
-      <c r="F63" s="64"/>
+      <c r="C63" s="59"/>
+      <c r="D63" s="49"/>
+      <c r="E63" s="50"/>
+      <c r="F63" s="51"/>
     </row>
     <row r="64" spans="3:6" ht="15" thickBot="1">
       <c r="C64" s="35"/>
       <c r="F64" s="7"/>
     </row>
     <row r="65" spans="3:6" ht="43.2">
-      <c r="C65" s="65" t="s">
+      <c r="C65" s="53" t="s">
         <v>229</v>
       </c>
-      <c r="D65" s="63"/>
-      <c r="E65" s="63" t="s">
+      <c r="D65" s="50"/>
+      <c r="E65" s="50" t="s">
         <v>230</v>
       </c>
-      <c r="F65" s="64" t="s">
+      <c r="F65" s="51" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="66" spans="3:6" ht="28.8">
-      <c r="C66" s="66"/>
-      <c r="D66" s="62" t="s">
+      <c r="C66" s="54"/>
+      <c r="D66" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="E66" s="63"/>
-      <c r="F66" s="64"/>
+      <c r="E66" s="50"/>
+      <c r="F66" s="51"/>
     </row>
     <row r="67" spans="3:6" ht="29.4" thickBot="1">
-      <c r="C67" s="69"/>
-      <c r="D67" s="62" t="s">
+      <c r="C67" s="59"/>
+      <c r="D67" s="49" t="s">
         <v>231</v>
       </c>
-      <c r="E67" s="63"/>
-      <c r="F67" s="64"/>
+      <c r="E67" s="50"/>
+      <c r="F67" s="51"/>
     </row>
     <row r="68" spans="3:6" ht="15" thickBot="1">
       <c r="C68" s="37"/>
       <c r="F68" s="7"/>
     </row>
     <row r="69" spans="3:6" ht="28.8">
-      <c r="C69" s="65" t="s">
+      <c r="C69" s="53" t="s">
         <v>232</v>
       </c>
-      <c r="D69" s="63"/>
-      <c r="E69" s="63" t="s">
+      <c r="D69" s="50"/>
+      <c r="E69" s="50" t="s">
         <v>233</v>
       </c>
-      <c r="F69" s="64" t="s">
+      <c r="F69" s="51" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="70" spans="3:6">
-      <c r="C70" s="66"/>
-      <c r="D70" s="62" t="s">
+      <c r="C70" s="54"/>
+      <c r="D70" s="49" t="s">
         <v>234</v>
       </c>
-      <c r="E70" s="63"/>
-      <c r="F70" s="64"/>
+      <c r="E70" s="50"/>
+      <c r="F70" s="51"/>
     </row>
     <row r="71" spans="3:6" ht="28.8">
-      <c r="C71" s="66"/>
-      <c r="D71" s="62" t="s">
+      <c r="C71" s="54"/>
+      <c r="D71" s="49" t="s">
         <v>235</v>
       </c>
-      <c r="E71" s="63"/>
-      <c r="F71" s="64"/>
+      <c r="E71" s="50"/>
+      <c r="F71" s="51"/>
     </row>
     <row r="72" spans="3:6">
-      <c r="C72" s="66"/>
-      <c r="D72" s="62" t="s">
+      <c r="C72" s="54"/>
+      <c r="D72" s="49" t="s">
         <v>236</v>
       </c>
-      <c r="E72" s="63"/>
-      <c r="F72" s="64"/>
+      <c r="E72" s="50"/>
+      <c r="F72" s="51"/>
     </row>
     <row r="73" spans="3:6" ht="15" thickBot="1">
-      <c r="C73" s="69"/>
-      <c r="D73" s="62" t="s">
+      <c r="C73" s="59"/>
+      <c r="D73" s="49" t="s">
         <v>237</v>
       </c>
-      <c r="E73" s="63"/>
-      <c r="F73" s="64"/>
+      <c r="E73" s="50"/>
+      <c r="F73" s="51"/>
     </row>
     <row r="74" spans="3:6" ht="15" thickBot="1">
       <c r="F74" s="7"/>
     </row>
     <row r="75" spans="3:6" ht="28.8">
-      <c r="C75" s="65" t="s">
+      <c r="C75" s="53" t="s">
         <v>260</v>
       </c>
-      <c r="D75" s="63"/>
-      <c r="E75" s="63" t="s">
+      <c r="D75" s="50"/>
+      <c r="E75" s="50" t="s">
         <v>233</v>
       </c>
-      <c r="F75" s="64" t="s">
+      <c r="F75" s="51" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="76" spans="3:6">
-      <c r="C76" s="66"/>
-      <c r="D76" s="62" t="s">
+      <c r="C76" s="54"/>
+      <c r="D76" s="49" t="s">
         <v>261</v>
       </c>
-      <c r="E76" s="63"/>
-      <c r="F76" s="64"/>
+      <c r="E76" s="50"/>
+      <c r="F76" s="51"/>
     </row>
     <row r="77" spans="3:6">
-      <c r="C77" s="66"/>
-      <c r="D77" s="62" t="s">
+      <c r="C77" s="54"/>
+      <c r="D77" s="49" t="s">
         <v>262</v>
       </c>
-      <c r="E77" s="63"/>
-      <c r="F77" s="64"/>
+      <c r="E77" s="50"/>
+      <c r="F77" s="51"/>
     </row>
     <row r="78" spans="3:6">
-      <c r="C78" s="66"/>
-      <c r="D78" s="62" t="s">
+      <c r="C78" s="54"/>
+      <c r="D78" s="49" t="s">
         <v>263</v>
       </c>
-      <c r="E78" s="63"/>
-      <c r="F78" s="64"/>
+      <c r="E78" s="50"/>
+      <c r="F78" s="51"/>
     </row>
     <row r="79" spans="3:6">
-      <c r="C79" s="66"/>
-      <c r="D79" s="62" t="s">
+      <c r="C79" s="54"/>
+      <c r="D79" s="49" t="s">
         <v>273</v>
       </c>
-      <c r="E79" s="63"/>
-      <c r="F79" s="64"/>
+      <c r="E79" s="50"/>
+      <c r="F79" s="51"/>
     </row>
     <row r="80" spans="3:6">
-      <c r="C80" s="66"/>
-      <c r="D80" s="62" t="s">
+      <c r="C80" s="54"/>
+      <c r="D80" s="49" t="s">
         <v>264</v>
       </c>
-      <c r="E80" s="63"/>
-      <c r="F80" s="64"/>
+      <c r="E80" s="50"/>
+      <c r="F80" s="51"/>
     </row>
     <row r="81" spans="3:6" ht="15" thickBot="1">
-      <c r="C81" s="69"/>
-      <c r="D81" s="62" t="s">
+      <c r="C81" s="59"/>
+      <c r="D81" s="49" t="s">
         <v>265</v>
       </c>
-      <c r="E81" s="63"/>
-      <c r="F81" s="64"/>
+      <c r="E81" s="50"/>
+      <c r="F81" s="51"/>
     </row>
     <row r="82" spans="3:6">
       <c r="F82" s="7"/>
@@ -2703,242 +2702,242 @@
       <c r="F83" s="7"/>
     </row>
     <row r="84" spans="3:6" ht="28.8">
-      <c r="C84" s="65" t="s">
+      <c r="C84" s="53" t="s">
         <v>167</v>
       </c>
-      <c r="D84" s="62"/>
-      <c r="E84" s="63" t="s">
+      <c r="D84" s="49"/>
+      <c r="E84" s="50" t="s">
         <v>183</v>
       </c>
-      <c r="F84" s="63"/>
+      <c r="F84" s="50"/>
     </row>
     <row r="85" spans="3:6" ht="237" customHeight="1">
-      <c r="C85" s="66"/>
-      <c r="D85" s="62" t="s">
+      <c r="C85" s="54"/>
+      <c r="D85" s="49" t="s">
         <v>181</v>
       </c>
-      <c r="E85" s="63" t="s">
+      <c r="E85" s="50" t="s">
         <v>184</v>
       </c>
-      <c r="F85" s="64"/>
+      <c r="F85" s="51"/>
     </row>
     <row r="86" spans="3:6" ht="43.2">
-      <c r="C86" s="66"/>
-      <c r="D86" s="62" t="s">
+      <c r="C86" s="54"/>
+      <c r="D86" s="49" t="s">
         <v>182</v>
       </c>
-      <c r="E86" s="63" t="s">
+      <c r="E86" s="50" t="s">
         <v>185</v>
       </c>
-      <c r="F86" s="63"/>
+      <c r="F86" s="50"/>
     </row>
     <row r="87" spans="3:6" ht="144">
-      <c r="C87" s="66"/>
-      <c r="D87" s="62" t="s">
+      <c r="C87" s="54"/>
+      <c r="D87" s="49" t="s">
         <v>171</v>
       </c>
-      <c r="E87" s="63" t="s">
+      <c r="E87" s="50" t="s">
         <v>186</v>
       </c>
-      <c r="F87" s="64" t="s">
+      <c r="F87" s="51" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="88" spans="3:6" ht="43.2">
-      <c r="C88" s="66"/>
-      <c r="D88" s="62" t="s">
+      <c r="C88" s="54"/>
+      <c r="D88" s="49" t="s">
         <v>168</v>
       </c>
-      <c r="E88" s="63" t="s">
+      <c r="E88" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="F88" s="63"/>
+      <c r="F88" s="50"/>
     </row>
     <row r="89" spans="3:6" ht="72">
-      <c r="C89" s="66"/>
-      <c r="D89" s="62" t="s">
+      <c r="C89" s="54"/>
+      <c r="D89" s="49" t="s">
         <v>169</v>
       </c>
-      <c r="E89" s="63" t="s">
+      <c r="E89" s="50" t="s">
         <v>189</v>
       </c>
-      <c r="F89" s="63"/>
+      <c r="F89" s="50"/>
     </row>
     <row r="90" spans="3:6" ht="43.2">
-      <c r="C90" s="66"/>
-      <c r="D90" s="62" t="s">
+      <c r="C90" s="54"/>
+      <c r="D90" s="49" t="s">
         <v>170</v>
       </c>
-      <c r="E90" s="63" t="s">
+      <c r="E90" s="50" t="s">
         <v>188</v>
       </c>
-      <c r="F90" s="63"/>
+      <c r="F90" s="50"/>
     </row>
     <row r="91" spans="3:6" ht="15" thickBot="1">
-      <c r="C91" s="67"/>
-      <c r="D91" s="62" t="s">
+      <c r="C91" s="55"/>
+      <c r="D91" s="49" t="s">
         <v>191</v>
       </c>
-      <c r="E91" s="63"/>
-      <c r="F91" s="63"/>
+      <c r="E91" s="50"/>
+      <c r="F91" s="50"/>
     </row>
     <row r="92" spans="3:6" ht="15" thickBot="1">
       <c r="E92" s="8"/>
     </row>
     <row r="93" spans="3:6" ht="43.2">
-      <c r="C93" s="65" t="s">
+      <c r="C93" s="53" t="s">
         <v>175</v>
       </c>
-      <c r="D93" s="62" t="s">
+      <c r="D93" s="49" t="s">
         <v>176</v>
       </c>
-      <c r="E93" s="63" t="s">
+      <c r="E93" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="F93" s="64" t="s">
+      <c r="F93" s="51" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="94" spans="3:6" ht="43.2">
-      <c r="C94" s="66"/>
-      <c r="D94" s="62" t="s">
+      <c r="C94" s="54"/>
+      <c r="D94" s="49" t="s">
         <v>172</v>
       </c>
-      <c r="E94" s="63" t="s">
+      <c r="E94" s="50" t="s">
         <v>247</v>
       </c>
-      <c r="F94" s="64" t="s">
+      <c r="F94" s="51" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="95" spans="3:6">
-      <c r="C95" s="66"/>
-      <c r="D95" s="62" t="s">
+      <c r="C95" s="54"/>
+      <c r="D95" s="49" t="s">
         <v>173</v>
       </c>
-      <c r="E95" s="70"/>
-      <c r="F95" s="64" t="s">
+      <c r="E95" s="52"/>
+      <c r="F95" s="51" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="96" spans="3:6">
-      <c r="C96" s="66"/>
-      <c r="D96" s="62" t="s">
+      <c r="C96" s="54"/>
+      <c r="D96" s="49" t="s">
         <v>180</v>
       </c>
-      <c r="E96" s="70"/>
-      <c r="F96" s="63"/>
+      <c r="E96" s="52"/>
+      <c r="F96" s="50"/>
     </row>
     <row r="97" spans="3:6">
-      <c r="C97" s="66"/>
-      <c r="D97" s="62" t="s">
+      <c r="C97" s="54"/>
+      <c r="D97" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="E97" s="70"/>
-      <c r="F97" s="63"/>
+      <c r="E97" s="52"/>
+      <c r="F97" s="50"/>
     </row>
     <row r="98" spans="3:6" ht="115.8" thickBot="1">
-      <c r="C98" s="67"/>
-      <c r="D98" s="62" t="s">
+      <c r="C98" s="55"/>
+      <c r="D98" s="49" t="s">
         <v>177</v>
       </c>
-      <c r="E98" s="63" t="s">
+      <c r="E98" s="50" t="s">
         <v>194</v>
       </c>
-      <c r="F98" s="63"/>
+      <c r="F98" s="50"/>
     </row>
     <row r="99" spans="3:6" ht="15" thickBot="1">
       <c r="E99" s="8"/>
     </row>
     <row r="100" spans="3:6">
-      <c r="C100" s="65" t="s">
+      <c r="C100" s="53" t="s">
         <v>174</v>
       </c>
-      <c r="D100" s="62" t="s">
+      <c r="D100" s="49" t="s">
         <v>178</v>
       </c>
-      <c r="E100" s="70"/>
-      <c r="F100" s="63"/>
+      <c r="E100" s="52"/>
+      <c r="F100" s="50"/>
     </row>
     <row r="101" spans="3:6">
-      <c r="C101" s="66"/>
-      <c r="D101" s="62" t="s">
+      <c r="C101" s="54"/>
+      <c r="D101" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="E101" s="70"/>
-      <c r="F101" s="63"/>
+      <c r="E101" s="52"/>
+      <c r="F101" s="50"/>
     </row>
     <row r="102" spans="3:6" ht="15" thickBot="1">
-      <c r="C102" s="67"/>
-      <c r="D102" s="62" t="s">
+      <c r="C102" s="55"/>
+      <c r="D102" s="49" t="s">
         <v>179</v>
       </c>
-      <c r="E102" s="70"/>
-      <c r="F102" s="63"/>
+      <c r="E102" s="52"/>
+      <c r="F102" s="50"/>
     </row>
     <row r="103" spans="3:6" ht="15" thickBot="1">
       <c r="E103" s="8"/>
     </row>
     <row r="104" spans="3:6" ht="28.8">
-      <c r="C104" s="65" t="s">
+      <c r="C104" s="53" t="s">
         <v>212</v>
       </c>
-      <c r="D104" s="62" t="s">
+      <c r="D104" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="E104" s="70"/>
-      <c r="F104" s="63"/>
+      <c r="E104" s="52"/>
+      <c r="F104" s="50"/>
     </row>
     <row r="105" spans="3:6" ht="28.8">
-      <c r="C105" s="66"/>
-      <c r="D105" s="62" t="s">
+      <c r="C105" s="54"/>
+      <c r="D105" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="E105" s="70"/>
-      <c r="F105" s="63"/>
+      <c r="E105" s="52"/>
+      <c r="F105" s="50"/>
     </row>
     <row r="106" spans="3:6" ht="29.4" thickBot="1">
-      <c r="C106" s="67"/>
-      <c r="D106" s="62" t="s">
+      <c r="C106" s="55"/>
+      <c r="D106" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="E106" s="70"/>
-      <c r="F106" s="63"/>
+      <c r="E106" s="52"/>
+      <c r="F106" s="50"/>
     </row>
     <row r="107" spans="3:6" ht="15" thickBot="1">
       <c r="E107" s="8"/>
     </row>
     <row r="108" spans="3:6" ht="72">
-      <c r="C108" s="65" t="s">
+      <c r="C108" s="53" t="s">
         <v>202</v>
       </c>
-      <c r="D108" s="62"/>
-      <c r="E108" s="70" t="s">
+      <c r="D108" s="49"/>
+      <c r="E108" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F108" s="64" t="s">
+      <c r="F108" s="51" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="109" spans="3:6" ht="115.2">
-      <c r="C109" s="66"/>
-      <c r="D109" s="62" t="s">
+      <c r="C109" s="54"/>
+      <c r="D109" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="E109" s="63" t="s">
+      <c r="E109" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="F109" s="64" t="s">
+      <c r="F109" s="51" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="110" spans="3:6" ht="15" thickBot="1">
-      <c r="C110" s="67"/>
-      <c r="D110" s="62" t="s">
+      <c r="C110" s="55"/>
+      <c r="D110" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="E110" s="63"/>
-      <c r="F110" s="64" t="s">
+      <c r="E110" s="50"/>
+      <c r="F110" s="51" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2994,54 +2993,54 @@
       </c>
     </row>
     <row r="118" spans="3:6" ht="144">
-      <c r="C118" s="71" t="s">
+      <c r="C118" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="D118" s="62" t="s">
+      <c r="D118" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="E118" s="63" t="s">
+      <c r="E118" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="F118" s="64" t="s">
+      <c r="F118" s="51" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="119" spans="3:6" ht="86.4">
-      <c r="C119" s="72"/>
-      <c r="D119" s="62" t="s">
+      <c r="C119" s="61"/>
+      <c r="D119" s="49" t="s">
         <v>147</v>
       </c>
-      <c r="E119" s="63" t="s">
+      <c r="E119" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="F119" s="64"/>
+      <c r="F119" s="51"/>
     </row>
     <row r="120" spans="3:6">
-      <c r="C120" s="72"/>
-      <c r="D120" s="62" t="s">
+      <c r="C120" s="61"/>
+      <c r="D120" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="E120" s="63"/>
-      <c r="F120" s="64"/>
+      <c r="E120" s="50"/>
+      <c r="F120" s="51"/>
     </row>
     <row r="121" spans="3:6" ht="43.2">
-      <c r="C121" s="72"/>
-      <c r="D121" s="62" t="s">
+      <c r="C121" s="61"/>
+      <c r="D121" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="E121" s="63"/>
-      <c r="F121" s="64" t="s">
+      <c r="E121" s="50"/>
+      <c r="F121" s="51" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="122" spans="3:6" ht="43.8" thickBot="1">
-      <c r="C122" s="73"/>
-      <c r="D122" s="62" t="s">
+      <c r="C122" s="62"/>
+      <c r="D122" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="E122" s="63"/>
-      <c r="F122" s="64" t="s">
+      <c r="E122" s="50"/>
+      <c r="F122" s="51" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3097,7 +3096,7 @@
       <c r="F128" s="7"/>
     </row>
     <row r="129" spans="3:6">
-      <c r="C129" s="48" t="s">
+      <c r="C129" s="56" t="s">
         <v>195</v>
       </c>
       <c r="D129" s="28" t="s">
@@ -3106,35 +3105,35 @@
       <c r="F129" s="7"/>
     </row>
     <row r="130" spans="3:6">
-      <c r="C130" s="49"/>
+      <c r="C130" s="63"/>
       <c r="D130" s="28" t="s">
         <v>196</v>
       </c>
       <c r="F130" s="7"/>
     </row>
     <row r="131" spans="3:6">
-      <c r="C131" s="49"/>
+      <c r="C131" s="63"/>
       <c r="D131" s="28" t="s">
         <v>198</v>
       </c>
       <c r="F131" s="7"/>
     </row>
     <row r="132" spans="3:6">
-      <c r="C132" s="49"/>
+      <c r="C132" s="63"/>
       <c r="D132" s="28" t="s">
         <v>199</v>
       </c>
       <c r="F132" s="7"/>
     </row>
     <row r="133" spans="3:6">
-      <c r="C133" s="49"/>
+      <c r="C133" s="63"/>
       <c r="D133" s="28" t="s">
         <v>200</v>
       </c>
       <c r="F133" s="7"/>
     </row>
     <row r="134" spans="3:6" ht="15" thickBot="1">
-      <c r="C134" s="50"/>
+      <c r="C134" s="64"/>
       <c r="D134" s="28" t="s">
         <v>201</v>
       </c>
@@ -3149,13 +3148,13 @@
       <c r="F136" s="7"/>
     </row>
     <row r="137" spans="3:6">
-      <c r="C137" s="48" t="s">
+      <c r="C137" s="56" t="s">
         <v>203</v>
       </c>
       <c r="F137" s="7"/>
     </row>
     <row r="138" spans="3:6" ht="15" thickBot="1">
-      <c r="C138" s="51"/>
+      <c r="C138" s="57"/>
       <c r="F138" s="7"/>
     </row>
     <row r="139" spans="3:6">
@@ -3314,6 +3313,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C108:C110"/>
+    <mergeCell ref="C75:C81"/>
     <mergeCell ref="C19:C24"/>
     <mergeCell ref="C137:C138"/>
     <mergeCell ref="C104:C106"/>
@@ -3330,8 +3331,6 @@
     <mergeCell ref="C93:C98"/>
     <mergeCell ref="C100:C102"/>
     <mergeCell ref="C129:C134"/>
-    <mergeCell ref="C108:C110"/>
-    <mergeCell ref="C75:C81"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F27" r:id="rId1"/>
@@ -3421,10 +3420,10 @@
       <c r="E3" s="13"/>
     </row>
     <row r="4" spans="2:5" ht="15">
-      <c r="B4" s="52">
+      <c r="B4" s="65">
         <v>1</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="66" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -3433,48 +3432,48 @@
       <c r="E4" s="13"/>
     </row>
     <row r="5" spans="2:5" ht="15">
-      <c r="B5" s="52"/>
-      <c r="C5" s="53"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="66"/>
       <c r="D5" s="15" t="s">
         <v>40</v>
       </c>
       <c r="E5" s="13"/>
     </row>
     <row r="6" spans="2:5" ht="15">
-      <c r="B6" s="52"/>
-      <c r="C6" s="53"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="15" t="s">
         <v>41</v>
       </c>
       <c r="E6" s="13"/>
     </row>
     <row r="7" spans="2:5" ht="15">
-      <c r="B7" s="52"/>
-      <c r="C7" s="53"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="66"/>
       <c r="D7" s="15" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="13"/>
     </row>
     <row r="8" spans="2:5" ht="15">
-      <c r="B8" s="52"/>
-      <c r="C8" s="53"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="66"/>
       <c r="D8" s="15" t="s">
         <v>43</v>
       </c>
       <c r="E8" s="13"/>
     </row>
     <row r="9" spans="2:5" ht="15">
-      <c r="B9" s="52"/>
-      <c r="C9" s="53"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="66"/>
       <c r="D9" s="15" t="s">
         <v>44</v>
       </c>
       <c r="E9" s="13"/>
     </row>
     <row r="10" spans="2:5" ht="15">
-      <c r="B10" s="52"/>
-      <c r="C10" s="53"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="15" t="s">
         <v>45</v>
       </c>
@@ -3487,10 +3486,10 @@
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="2:5" ht="15">
-      <c r="B12" s="52">
+      <c r="B12" s="65">
         <v>2</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="66" t="s">
         <v>46</v>
       </c>
       <c r="D12" s="13" t="s">
@@ -3501,8 +3500,8 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="15">
-      <c r="B13" s="52"/>
-      <c r="C13" s="53"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="66"/>
       <c r="D13" s="13" t="s">
         <v>49</v>
       </c>
@@ -3511,8 +3510,8 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="15">
-      <c r="B14" s="52"/>
-      <c r="C14" s="53"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="66"/>
       <c r="D14" s="13" t="s">
         <v>51</v>
       </c>
@@ -3525,10 +3524,10 @@
       <c r="E15" s="13"/>
     </row>
     <row r="16" spans="2:5" ht="15">
-      <c r="B16" s="54">
+      <c r="B16" s="67">
         <v>3</v>
       </c>
-      <c r="C16" s="57" t="s">
+      <c r="C16" s="69" t="s">
         <v>52</v>
       </c>
       <c r="D16" s="13" t="s">
@@ -3537,8 +3536,8 @@
       <c r="E16" s="13"/>
     </row>
     <row r="17" spans="2:5" ht="15">
-      <c r="B17" s="56"/>
-      <c r="C17" s="59"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="70"/>
       <c r="D17" s="13" t="s">
         <v>54</v>
       </c>
@@ -3551,10 +3550,10 @@
       <c r="E18" s="13"/>
     </row>
     <row r="19" spans="2:5" ht="15">
-      <c r="B19" s="52">
+      <c r="B19" s="65">
         <v>4</v>
       </c>
-      <c r="C19" s="53" t="s">
+      <c r="C19" s="66" t="s">
         <v>55</v>
       </c>
       <c r="D19" s="13" t="s">
@@ -3563,8 +3562,8 @@
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="2:5" ht="15">
-      <c r="B20" s="52"/>
-      <c r="C20" s="53"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="66"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
     </row>
@@ -3591,7 +3590,7 @@
       <c r="E23" s="13"/>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="54">
+      <c r="B24" s="67">
         <v>6</v>
       </c>
       <c r="C24" s="12" t="s">
@@ -3601,7 +3600,7 @@
       <c r="E24" s="13"/>
     </row>
     <row r="25" spans="2:5" ht="30">
-      <c r="B25" s="55"/>
+      <c r="B25" s="71"/>
       <c r="C25" s="12"/>
       <c r="D25" s="13" t="s">
         <v>59</v>
@@ -3609,14 +3608,14 @@
       <c r="E25" s="13"/>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="55"/>
+      <c r="B26" s="71"/>
       <c r="C26" s="12"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
     </row>
     <row r="27" spans="2:5" ht="15">
-      <c r="B27" s="55"/>
-      <c r="C27" s="57" t="s">
+      <c r="B27" s="71"/>
+      <c r="C27" s="69" t="s">
         <v>60</v>
       </c>
       <c r="D27" s="18" t="s">
@@ -3625,86 +3624,86 @@
       <c r="E27" s="13"/>
     </row>
     <row r="28" spans="2:5" ht="15">
-      <c r="B28" s="55"/>
-      <c r="C28" s="58"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="72"/>
       <c r="D28" s="18" t="s">
         <v>62</v>
       </c>
       <c r="E28" s="13"/>
     </row>
     <row r="29" spans="2:5" ht="15">
-      <c r="B29" s="55"/>
-      <c r="C29" s="58"/>
+      <c r="B29" s="71"/>
+      <c r="C29" s="72"/>
       <c r="D29" s="18" t="s">
         <v>63</v>
       </c>
       <c r="E29" s="13"/>
     </row>
     <row r="30" spans="2:5" ht="15">
-      <c r="B30" s="55"/>
-      <c r="C30" s="58"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="72"/>
       <c r="D30" s="18" t="s">
         <v>64</v>
       </c>
       <c r="E30" s="13"/>
     </row>
     <row r="31" spans="2:5" ht="15">
-      <c r="B31" s="55"/>
-      <c r="C31" s="58"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="72"/>
       <c r="D31" s="18" t="s">
         <v>65</v>
       </c>
       <c r="E31" s="13"/>
     </row>
     <row r="32" spans="2:5" ht="15">
-      <c r="B32" s="55"/>
-      <c r="C32" s="58"/>
+      <c r="B32" s="71"/>
+      <c r="C32" s="72"/>
       <c r="D32" s="18" t="s">
         <v>66</v>
       </c>
       <c r="E32" s="13"/>
     </row>
     <row r="33" spans="2:5" ht="15">
-      <c r="B33" s="55"/>
-      <c r="C33" s="58"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="72"/>
       <c r="D33" s="18" t="s">
         <v>67</v>
       </c>
       <c r="E33" s="13"/>
     </row>
     <row r="34" spans="2:5" ht="15">
-      <c r="B34" s="55"/>
-      <c r="C34" s="58"/>
+      <c r="B34" s="71"/>
+      <c r="C34" s="72"/>
       <c r="D34" s="18" t="s">
         <v>68</v>
       </c>
       <c r="E34" s="19"/>
     </row>
     <row r="35" spans="2:5" ht="15">
-      <c r="B35" s="55"/>
-      <c r="C35" s="58"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="72"/>
       <c r="D35" s="18" t="s">
         <v>69</v>
       </c>
       <c r="E35" s="13"/>
     </row>
     <row r="36" spans="2:5" ht="15">
-      <c r="B36" s="55"/>
-      <c r="C36" s="59"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="70"/>
       <c r="D36" s="13" t="s">
         <v>70</v>
       </c>
       <c r="E36" s="13"/>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="55"/>
+      <c r="B37" s="71"/>
       <c r="C37" s="12"/>
       <c r="D37" s="13"/>
       <c r="E37" s="13"/>
     </row>
     <row r="38" spans="2:5" ht="30">
-      <c r="B38" s="55"/>
-      <c r="C38" s="57" t="s">
+      <c r="B38" s="71"/>
+      <c r="C38" s="69" t="s">
         <v>71</v>
       </c>
       <c r="D38" s="13"/>
@@ -3713,38 +3712,38 @@
       </c>
     </row>
     <row r="39" spans="2:5" ht="15">
-      <c r="B39" s="55"/>
-      <c r="C39" s="60"/>
+      <c r="B39" s="71"/>
+      <c r="C39" s="73"/>
       <c r="D39" s="13"/>
       <c r="E39" s="16" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="40" spans="2:5">
-      <c r="B40" s="55"/>
+      <c r="B40" s="71"/>
       <c r="C40" s="12"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="56"/>
+      <c r="B41" s="68"/>
       <c r="C41" s="12"/>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B24:B41"/>
+    <mergeCell ref="C27:C36"/>
+    <mergeCell ref="C38:C39"/>
     <mergeCell ref="B4:B10"/>
     <mergeCell ref="C4:C10"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B24:B41"/>
-    <mergeCell ref="C27:C36"/>
-    <mergeCell ref="C38:C39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E13" r:id="rId1"/>

</xml_diff>

<commit_message>
DL notes is updated
</commit_message>
<xml_diff>
--- a/Learning_Topics.xlsx
+++ b/Learning_Topics.xlsx
@@ -1581,6 +1581,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1590,9 +1593,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1617,19 +1617,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1989,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -2389,7 +2389,7 @@
       </c>
     </row>
     <row r="44" spans="3:6" ht="115.2">
-      <c r="C44" s="58"/>
+      <c r="C44" s="59"/>
       <c r="D44" s="49" t="s">
         <v>205</v>
       </c>
@@ -2401,7 +2401,7 @@
       </c>
     </row>
     <row r="45" spans="3:6" ht="29.4" thickBot="1">
-      <c r="C45" s="59"/>
+      <c r="C45" s="56"/>
       <c r="D45" s="49" t="s">
         <v>216</v>
       </c>
@@ -2449,7 +2449,7 @@
       <c r="F50" s="51"/>
     </row>
     <row r="51" spans="3:6" ht="43.8" thickBot="1">
-      <c r="C51" s="59"/>
+      <c r="C51" s="56"/>
       <c r="D51" s="49" t="s">
         <v>269</v>
       </c>
@@ -2483,7 +2483,7 @@
       <c r="F54" s="51"/>
     </row>
     <row r="55" spans="3:6" ht="15" thickBot="1">
-      <c r="C55" s="59"/>
+      <c r="C55" s="56"/>
       <c r="D55" s="49" t="s">
         <v>223</v>
       </c>
@@ -2517,7 +2517,7 @@
       <c r="F58" s="51"/>
     </row>
     <row r="59" spans="3:6" ht="15" thickBot="1">
-      <c r="C59" s="59"/>
+      <c r="C59" s="56"/>
       <c r="D59" s="49"/>
       <c r="E59" s="50"/>
       <c r="F59" s="51"/>
@@ -2547,7 +2547,7 @@
       <c r="F62" s="51"/>
     </row>
     <row r="63" spans="3:6" ht="15" thickBot="1">
-      <c r="C63" s="59"/>
+      <c r="C63" s="56"/>
       <c r="D63" s="49"/>
       <c r="E63" s="50"/>
       <c r="F63" s="51"/>
@@ -2577,7 +2577,7 @@
       <c r="F66" s="51"/>
     </row>
     <row r="67" spans="3:6" ht="29.4" thickBot="1">
-      <c r="C67" s="59"/>
+      <c r="C67" s="56"/>
       <c r="D67" s="49" t="s">
         <v>231</v>
       </c>
@@ -2625,7 +2625,7 @@
       <c r="F72" s="51"/>
     </row>
     <row r="73" spans="3:6" ht="15" thickBot="1">
-      <c r="C73" s="59"/>
+      <c r="C73" s="56"/>
       <c r="D73" s="49" t="s">
         <v>237</v>
       </c>
@@ -2688,7 +2688,7 @@
       <c r="F80" s="51"/>
     </row>
     <row r="81" spans="3:6" ht="15" thickBot="1">
-      <c r="C81" s="59"/>
+      <c r="C81" s="56"/>
       <c r="D81" s="49" t="s">
         <v>265</v>
       </c>
@@ -3096,7 +3096,7 @@
       <c r="F128" s="7"/>
     </row>
     <row r="129" spans="3:6">
-      <c r="C129" s="56" t="s">
+      <c r="C129" s="57" t="s">
         <v>195</v>
       </c>
       <c r="D129" s="28" t="s">
@@ -3148,13 +3148,13 @@
       <c r="F136" s="7"/>
     </row>
     <row r="137" spans="3:6">
-      <c r="C137" s="56" t="s">
+      <c r="C137" s="57" t="s">
         <v>203</v>
       </c>
       <c r="F137" s="7"/>
     </row>
     <row r="138" spans="3:6" ht="15" thickBot="1">
-      <c r="C138" s="57"/>
+      <c r="C138" s="58"/>
       <c r="F138" s="7"/>
     </row>
     <row r="139" spans="3:6">
@@ -3313,6 +3313,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C100:C102"/>
+    <mergeCell ref="C129:C134"/>
     <mergeCell ref="C108:C110"/>
     <mergeCell ref="C75:C81"/>
     <mergeCell ref="C19:C24"/>
@@ -3329,8 +3331,6 @@
     <mergeCell ref="C31:C39"/>
     <mergeCell ref="C84:C91"/>
     <mergeCell ref="C93:C98"/>
-    <mergeCell ref="C100:C102"/>
-    <mergeCell ref="C129:C134"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F27" r:id="rId1"/>
@@ -3527,7 +3527,7 @@
       <c r="B16" s="67">
         <v>3</v>
       </c>
-      <c r="C16" s="69" t="s">
+      <c r="C16" s="70" t="s">
         <v>52</v>
       </c>
       <c r="D16" s="13" t="s">
@@ -3536,8 +3536,8 @@
       <c r="E16" s="13"/>
     </row>
     <row r="17" spans="2:5" ht="15">
-      <c r="B17" s="68"/>
-      <c r="C17" s="70"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="72"/>
       <c r="D17" s="13" t="s">
         <v>54</v>
       </c>
@@ -3600,7 +3600,7 @@
       <c r="E24" s="13"/>
     </row>
     <row r="25" spans="2:5" ht="30">
-      <c r="B25" s="71"/>
+      <c r="B25" s="68"/>
       <c r="C25" s="12"/>
       <c r="D25" s="13" t="s">
         <v>59</v>
@@ -3608,14 +3608,14 @@
       <c r="E25" s="13"/>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="71"/>
+      <c r="B26" s="68"/>
       <c r="C26" s="12"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
     </row>
     <row r="27" spans="2:5" ht="15">
-      <c r="B27" s="71"/>
-      <c r="C27" s="69" t="s">
+      <c r="B27" s="68"/>
+      <c r="C27" s="70" t="s">
         <v>60</v>
       </c>
       <c r="D27" s="18" t="s">
@@ -3624,86 +3624,86 @@
       <c r="E27" s="13"/>
     </row>
     <row r="28" spans="2:5" ht="15">
-      <c r="B28" s="71"/>
-      <c r="C28" s="72"/>
+      <c r="B28" s="68"/>
+      <c r="C28" s="71"/>
       <c r="D28" s="18" t="s">
         <v>62</v>
       </c>
       <c r="E28" s="13"/>
     </row>
     <row r="29" spans="2:5" ht="15">
-      <c r="B29" s="71"/>
-      <c r="C29" s="72"/>
+      <c r="B29" s="68"/>
+      <c r="C29" s="71"/>
       <c r="D29" s="18" t="s">
         <v>63</v>
       </c>
       <c r="E29" s="13"/>
     </row>
     <row r="30" spans="2:5" ht="15">
-      <c r="B30" s="71"/>
-      <c r="C30" s="72"/>
+      <c r="B30" s="68"/>
+      <c r="C30" s="71"/>
       <c r="D30" s="18" t="s">
         <v>64</v>
       </c>
       <c r="E30" s="13"/>
     </row>
     <row r="31" spans="2:5" ht="15">
-      <c r="B31" s="71"/>
-      <c r="C31" s="72"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="71"/>
       <c r="D31" s="18" t="s">
         <v>65</v>
       </c>
       <c r="E31" s="13"/>
     </row>
     <row r="32" spans="2:5" ht="15">
-      <c r="B32" s="71"/>
-      <c r="C32" s="72"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="71"/>
       <c r="D32" s="18" t="s">
         <v>66</v>
       </c>
       <c r="E32" s="13"/>
     </row>
     <row r="33" spans="2:5" ht="15">
-      <c r="B33" s="71"/>
-      <c r="C33" s="72"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="71"/>
       <c r="D33" s="18" t="s">
         <v>67</v>
       </c>
       <c r="E33" s="13"/>
     </row>
     <row r="34" spans="2:5" ht="15">
-      <c r="B34" s="71"/>
-      <c r="C34" s="72"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="71"/>
       <c r="D34" s="18" t="s">
         <v>68</v>
       </c>
       <c r="E34" s="19"/>
     </row>
     <row r="35" spans="2:5" ht="15">
-      <c r="B35" s="71"/>
-      <c r="C35" s="72"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="71"/>
       <c r="D35" s="18" t="s">
         <v>69</v>
       </c>
       <c r="E35" s="13"/>
     </row>
     <row r="36" spans="2:5" ht="15">
-      <c r="B36" s="71"/>
-      <c r="C36" s="70"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="72"/>
       <c r="D36" s="13" t="s">
         <v>70</v>
       </c>
       <c r="E36" s="13"/>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="71"/>
+      <c r="B37" s="68"/>
       <c r="C37" s="12"/>
       <c r="D37" s="13"/>
       <c r="E37" s="13"/>
     </row>
     <row r="38" spans="2:5" ht="30">
-      <c r="B38" s="71"/>
-      <c r="C38" s="69" t="s">
+      <c r="B38" s="68"/>
+      <c r="C38" s="70" t="s">
         <v>71</v>
       </c>
       <c r="D38" s="13"/>
@@ -3712,7 +3712,7 @@
       </c>
     </row>
     <row r="39" spans="2:5" ht="15">
-      <c r="B39" s="71"/>
+      <c r="B39" s="68"/>
       <c r="C39" s="73"/>
       <c r="D39" s="13"/>
       <c r="E39" s="16" t="s">
@@ -3720,30 +3720,30 @@
       </c>
     </row>
     <row r="40" spans="2:5">
-      <c r="B40" s="71"/>
+      <c r="B40" s="68"/>
       <c r="C40" s="12"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="68"/>
+      <c r="B41" s="69"/>
       <c r="C41" s="12"/>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B24:B41"/>
-    <mergeCell ref="C27:C36"/>
-    <mergeCell ref="C38:C39"/>
     <mergeCell ref="B4:B10"/>
     <mergeCell ref="C4:C10"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B24:B41"/>
+    <mergeCell ref="C27:C36"/>
+    <mergeCell ref="C38:C39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E13" r:id="rId1"/>

</xml_diff>